<commit_message>
Update parameters and add sensitivity analysis
</commit_message>
<xml_diff>
--- a/output/supp_mat1.xlsx
+++ b/output/supp_mat1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Species</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t xml:space="preserve">Beta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of days of release during a year</t>
   </si>
   <si>
     <t xml:space="preserve">E</t>
@@ -553,22 +550,22 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>0.700000579981133</v>
+        <v>0.700001811236143</v>
       </c>
       <c r="C6" t="n">
-        <v>0.705002268069657</v>
+        <v>0.70496788044693</v>
       </c>
       <c r="D6" t="n">
-        <v>0.800025819205955</v>
+        <v>0.80007383994121</v>
       </c>
       <c r="E6" t="n">
-        <v>0.799708862253465</v>
+        <v>0.800271685374901</v>
       </c>
       <c r="F6" t="n">
-        <v>0.895056585909333</v>
+        <v>0.895090315255802</v>
       </c>
       <c r="G6" t="n">
-        <v>0.899998579220846</v>
+        <v>0.899998423038051</v>
       </c>
       <c r="H6" t="s">
         <v>13</v>
@@ -579,22 +576,22 @@
         <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>0.700002903211862</v>
+        <v>0.700001150928438</v>
       </c>
       <c r="C7" t="n">
-        <v>0.705050308435457</v>
+        <v>0.705093145510182</v>
       </c>
       <c r="D7" t="n">
-        <v>0.799993494319205</v>
+        <v>0.799647583791757</v>
       </c>
       <c r="E7" t="n">
-        <v>0.800009856349789</v>
+        <v>0.79933705937583</v>
       </c>
       <c r="F7" t="n">
-        <v>0.894995604254073</v>
+        <v>0.895062818252481</v>
       </c>
       <c r="G7" t="n">
-        <v>0.899999898858368</v>
+        <v>0.899995928537101</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
@@ -605,22 +602,22 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>0.700001811236143</v>
+        <v>0.700000837771222</v>
       </c>
       <c r="C8" t="n">
-        <v>0.704944445467554</v>
+        <v>0.705081279155566</v>
       </c>
       <c r="D8" t="n">
-        <v>0.800033641652898</v>
+        <v>0.800030204583919</v>
       </c>
       <c r="E8" t="n">
-        <v>0.800292727490887</v>
+        <v>0.799941926635802</v>
       </c>
       <c r="F8" t="n">
-        <v>0.895041146902368</v>
+        <v>0.895009273065953</v>
       </c>
       <c r="G8" t="n">
-        <v>0.899998423038051</v>
+        <v>0.899999898858368</v>
       </c>
       <c r="H8" t="s">
         <v>13</v>
@@ -631,22 +628,22 @@
         <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>0.700000837771222</v>
+        <v>0.700002903211862</v>
       </c>
       <c r="C9" t="n">
-        <v>0.70505321525503</v>
+        <v>0.705080787969055</v>
       </c>
       <c r="D9" t="n">
-        <v>0.800016172679191</v>
+        <v>0.800366981181518</v>
       </c>
       <c r="E9" t="n">
-        <v>0.799873375031166</v>
+        <v>0.800514999125153</v>
       </c>
       <c r="F9" t="n">
-        <v>0.894968028911389</v>
+        <v>0.894994616878685</v>
       </c>
       <c r="G9" t="n">
-        <v>0.899996816599742</v>
+        <v>0.89999964335002</v>
       </c>
       <c r="H9" t="s">
         <v>13</v>
@@ -657,22 +654,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>29.8058371539987</v>
+        <v>150.181160860824</v>
       </c>
       <c r="C10" t="n">
-        <v>209.282977920802</v>
+        <v>216.239930707766</v>
       </c>
       <c r="D10" t="n">
-        <v>343.008925193269</v>
+        <v>350.439790347815</v>
       </c>
       <c r="E10" t="n">
-        <v>342.914689033067</v>
+        <v>350.090153254699</v>
       </c>
       <c r="F10" t="n">
-        <v>477.741490309317</v>
+        <v>487.370085649412</v>
       </c>
       <c r="G10" t="n">
-        <v>650.2677262005</v>
+        <v>598.954752538631</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
@@ -683,22 +680,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>49.2743360475802</v>
+        <v>120.125352176326</v>
       </c>
       <c r="C11" t="n">
-        <v>153.364470985682</v>
+        <v>183.730836474826</v>
       </c>
       <c r="D11" t="n">
-        <v>251.918977051926</v>
+        <v>300.130480623288</v>
       </c>
       <c r="E11" t="n">
-        <v>251.853713291848</v>
+        <v>299.863312968684</v>
       </c>
       <c r="F11" t="n">
-        <v>350.757106443517</v>
+        <v>417.464142632563</v>
       </c>
       <c r="G11" t="n">
-        <v>463.470506129</v>
+        <v>551.750602534524</v>
       </c>
       <c r="H11" t="s">
         <v>14</v>
@@ -709,22 +706,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>23.3521396214448</v>
+        <v>120.012006285658</v>
       </c>
       <c r="C12" t="n">
-        <v>107.094772640288</v>
+        <v>133.165556370266</v>
       </c>
       <c r="D12" t="n">
-        <v>176.937575617468</v>
+        <v>202.233834924678</v>
       </c>
       <c r="E12" t="n">
-        <v>177.019429065528</v>
+        <v>201.305058421491</v>
       </c>
       <c r="F12" t="n">
-        <v>246.391046896958</v>
+        <v>278.765796567236</v>
       </c>
       <c r="G12" t="n">
-        <v>335.404393403387</v>
+        <v>378.98801514507</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
@@ -735,22 +732,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>11.9434432539728</v>
+        <v>100.004433526833</v>
       </c>
       <c r="C13" t="n">
-        <v>95.8621543216271</v>
+        <v>108.6010624432</v>
       </c>
       <c r="D13" t="n">
-        <v>157.828462299083</v>
+        <v>161.879178311019</v>
       </c>
       <c r="E13" t="n">
-        <v>157.837433274228</v>
+        <v>160.94484622727</v>
       </c>
       <c r="F13" t="n">
-        <v>219.877341349994</v>
+        <v>222.042381346297</v>
       </c>
       <c r="G13" t="n">
-        <v>286.207152226026</v>
+        <v>249.991749570722</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
@@ -761,22 +758,22 @@
         <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>0.602136799134643</v>
+        <v>2.00006225495175</v>
       </c>
       <c r="C14" t="n">
-        <v>2.0199152592962</v>
+        <v>2.1635568070267</v>
       </c>
       <c r="D14" t="n">
-        <v>2.99924750458052</v>
+        <v>2.99985416289308</v>
       </c>
       <c r="E14" t="n">
-        <v>2.99944296988328</v>
+        <v>3.00078225021505</v>
       </c>
       <c r="F14" t="n">
-        <v>3.97577844078552</v>
+        <v>3.83738228851313</v>
       </c>
       <c r="G14" t="n">
-        <v>5.3707302454242</v>
+        <v>3.99998510921555</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -787,22 +784,22 @@
         <v>10</v>
       </c>
       <c r="B15" t="n">
-        <v>0.567850578890226</v>
+        <v>1.50003185815246</v>
       </c>
       <c r="C15" t="n">
-        <v>2.02396554777402</v>
+        <v>1.54173246736505</v>
       </c>
       <c r="D15" t="n">
-        <v>2.99853700554301</v>
+        <v>2.13934198280267</v>
       </c>
       <c r="E15" t="n">
-        <v>2.99815364480205</v>
+        <v>2.09676970067916</v>
       </c>
       <c r="F15" t="n">
-        <v>3.97201851204226</v>
+        <v>2.99748874673924</v>
       </c>
       <c r="G15" t="n">
-        <v>5.04032967418156</v>
+        <v>3.49674421285102</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -813,22 +810,22 @@
         <v>11</v>
       </c>
       <c r="B16" t="n">
-        <v>0.866260512947109</v>
+        <v>1.50000109295336</v>
       </c>
       <c r="C16" t="n">
-        <v>2.02032914100901</v>
+        <v>1.54155441498648</v>
       </c>
       <c r="D16" t="n">
-        <v>3.00225560846732</v>
+        <v>2.14328752820788</v>
       </c>
       <c r="E16" t="n">
-        <v>3.00449812790068</v>
+        <v>2.1023006098673</v>
       </c>
       <c r="F16" t="n">
-        <v>3.9785298578232</v>
+        <v>2.99654669463597</v>
       </c>
       <c r="G16" t="n">
-        <v>5.18403843739945</v>
+        <v>3.49656624052573</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -839,22 +836,22 @@
         <v>12</v>
       </c>
       <c r="B17" t="n">
-        <v>0.791617187284692</v>
+        <v>1.50004026131774</v>
       </c>
       <c r="C17" t="n">
-        <v>2.01555058591649</v>
+        <v>1.54199366376834</v>
       </c>
       <c r="D17" t="n">
-        <v>2.999022572869</v>
+        <v>2.13980822488899</v>
       </c>
       <c r="E17" t="n">
-        <v>2.99969595791537</v>
+        <v>2.09793774222279</v>
       </c>
       <c r="F17" t="n">
-        <v>3.96995916224729</v>
+        <v>2.99951777249164</v>
       </c>
       <c r="G17" t="n">
-        <v>5.14193781240708</v>
+        <v>3.49778979124242</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -865,22 +862,22 @@
         <v>8</v>
       </c>
       <c r="B18" t="n">
-        <v>325.00054615899</v>
+        <v>-255.607673324276</v>
       </c>
       <c r="C18" t="n">
-        <v>325.892886943038</v>
+        <v>4052.61644416774</v>
       </c>
       <c r="D18" t="n">
-        <v>342.512667930922</v>
+        <v>6685.56575428907</v>
       </c>
       <c r="E18" t="n">
-        <v>342.525582318194</v>
+        <v>6684.41404528326</v>
       </c>
       <c r="F18" t="n">
-        <v>359.124676951411</v>
+        <v>9313.88715384222</v>
       </c>
       <c r="G18" t="n">
-        <v>359.999841524987</v>
+        <v>12681.0377219363</v>
       </c>
       <c r="H18" t="s">
         <v>16</v>
@@ -891,22 +888,22 @@
         <v>10</v>
       </c>
       <c r="B19" t="n">
-        <v>325.000003658934</v>
+        <v>30.634125933163</v>
       </c>
       <c r="C19" t="n">
-        <v>325.862275737862</v>
+        <v>3263.87668454254</v>
       </c>
       <c r="D19" t="n">
-        <v>342.540069838944</v>
+        <v>5384.08191592643</v>
       </c>
       <c r="E19" t="n">
-        <v>342.546667802962</v>
+        <v>5387.51432937277</v>
       </c>
       <c r="F19" t="n">
-        <v>359.151415340835</v>
+        <v>7488.66046736652</v>
       </c>
       <c r="G19" t="n">
-        <v>359.998973176116</v>
+        <v>10165.5014233408</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
@@ -917,22 +914,22 @@
         <v>11</v>
       </c>
       <c r="B20" t="n">
-        <v>325.000201412477</v>
+        <v>1149.99784016005</v>
       </c>
       <c r="C20" t="n">
-        <v>325.894400895253</v>
+        <v>3100.89699900894</v>
       </c>
       <c r="D20" t="n">
-        <v>342.489577996086</v>
+        <v>5107.59670316838</v>
       </c>
       <c r="E20" t="n">
-        <v>342.444982506568</v>
+        <v>5106.78421094146</v>
       </c>
       <c r="F20" t="n">
-        <v>359.145753467514</v>
+        <v>7113.05192640197</v>
       </c>
       <c r="G20" t="n">
-        <v>359.999626650242</v>
+        <v>9576.0876904207</v>
       </c>
       <c r="H20" t="s">
         <v>16</v>
@@ -943,22 +940,22 @@
         <v>12</v>
       </c>
       <c r="B21" t="n">
-        <v>325.00022914377</v>
+        <v>262.088922644303</v>
       </c>
       <c r="C21" t="n">
-        <v>325.847878732719</v>
+        <v>2925.47308240002</v>
       </c>
       <c r="D21" t="n">
-        <v>342.499470987616</v>
+        <v>4793.01324790698</v>
       </c>
       <c r="E21" t="n">
-        <v>342.519751286018</v>
+        <v>4789.30792632583</v>
       </c>
       <c r="F21" t="n">
-        <v>359.135030381265</v>
+        <v>6680.1025739565</v>
       </c>
       <c r="G21" t="n">
-        <v>359.999870869797</v>
+        <v>8955.38754266021</v>
       </c>
       <c r="H21" t="s">
         <v>16</v>
@@ -969,22 +966,22 @@
         <v>8</v>
       </c>
       <c r="B22" t="n">
-        <v>365.518852818848</v>
+        <v>6.21190658223515</v>
       </c>
       <c r="C22" t="n">
-        <v>4065.77649559465</v>
+        <v>40.9434406252643</v>
       </c>
       <c r="D22" t="n">
-        <v>6678.54405799358</v>
+        <v>67.4672383051028</v>
       </c>
       <c r="E22" t="n">
-        <v>6677.17260280179</v>
+        <v>67.4697795709903</v>
       </c>
       <c r="F22" t="n">
-        <v>9303.83437277963</v>
+        <v>93.7327110703161</v>
       </c>
       <c r="G22" t="n">
-        <v>12523.8400418778</v>
+        <v>125.211840917443</v>
       </c>
       <c r="H22" t="s">
         <v>17</v>
@@ -995,22 +992,22 @@
         <v>10</v>
       </c>
       <c r="B23" t="n">
-        <v>978.20686344311</v>
+        <v>1.19770314820292</v>
       </c>
       <c r="C23" t="n">
-        <v>3269.67663600077</v>
+        <v>13.7763234290124</v>
       </c>
       <c r="D23" t="n">
-        <v>5380.81928835388</v>
+        <v>22.644500831395</v>
       </c>
       <c r="E23" t="n">
-        <v>5379.31041760352</v>
+        <v>22.6413987061968</v>
       </c>
       <c r="F23" t="n">
-        <v>7489.6345660939</v>
+        <v>31.4609650185001</v>
       </c>
       <c r="G23" t="n">
-        <v>9984.16726304676</v>
+        <v>44.3854201128228</v>
       </c>
       <c r="H23" t="s">
         <v>17</v>
@@ -1021,22 +1018,22 @@
         <v>11</v>
       </c>
       <c r="B24" t="n">
-        <v>374.133851181417</v>
+        <v>2.65500582636507</v>
       </c>
       <c r="C24" t="n">
-        <v>3101.67675491645</v>
+        <v>6.90623673321767</v>
       </c>
       <c r="D24" t="n">
-        <v>5109.27565536895</v>
+        <v>11.4118816556038</v>
       </c>
       <c r="E24" t="n">
-        <v>5107.72128983765</v>
+        <v>11.410716304163</v>
       </c>
       <c r="F24" t="n">
-        <v>7113.14892516447</v>
+        <v>15.8941206910778</v>
       </c>
       <c r="G24" t="n">
-        <v>9549.84017452924</v>
+        <v>20.6577067033601</v>
       </c>
       <c r="H24" t="s">
         <v>17</v>
@@ -1047,22 +1044,22 @@
         <v>12</v>
       </c>
       <c r="B25" t="n">
-        <v>27.2791630137945</v>
+        <v>1.84386003898119</v>
       </c>
       <c r="C25" t="n">
-        <v>2913.10345128088</v>
+        <v>9.74663716322788</v>
       </c>
       <c r="D25" t="n">
-        <v>4794.67386072614</v>
+        <v>16.0455995929792</v>
       </c>
       <c r="E25" t="n">
-        <v>4796.97841541369</v>
+        <v>16.0586339574205</v>
       </c>
       <c r="F25" t="n">
-        <v>6663.27742389517</v>
+        <v>22.3210506774854</v>
       </c>
       <c r="G25" t="n">
-        <v>9052.20442878959</v>
+        <v>29.6548001554127</v>
       </c>
       <c r="H25" t="s">
         <v>17</v>
@@ -1073,22 +1070,22 @@
         <v>8</v>
       </c>
       <c r="B26" t="n">
-        <v>9.12370426519021</v>
+        <v>-0.939230566483178</v>
       </c>
       <c r="C26" t="n">
-        <v>40.8413698184694</v>
+        <v>0.0209240299900077</v>
       </c>
       <c r="D26" t="n">
-        <v>67.5138277256514</v>
+        <v>0.0355947208993608</v>
       </c>
       <c r="E26" t="n">
-        <v>67.5491814106837</v>
+        <v>0.033980564930037</v>
       </c>
       <c r="F26" t="n">
-        <v>93.9780615995324</v>
+        <v>0.0598677409750342</v>
       </c>
       <c r="G26" t="n">
-        <v>123.445683852867</v>
+        <v>0.226473626458116</v>
       </c>
       <c r="H26" t="s">
         <v>18</v>
@@ -1096,470 +1093,470 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B27" t="n">
-        <v>3.72973093188677</v>
+        <v>25609.6391427034</v>
       </c>
       <c r="C27" t="n">
-        <v>13.7536573357153</v>
+        <v>44065.4880345249</v>
       </c>
       <c r="D27" t="n">
-        <v>22.6316748158766</v>
+        <v>70953.2529705163</v>
       </c>
       <c r="E27" t="n">
-        <v>22.6277851823903</v>
+        <v>70235.8051846787</v>
       </c>
       <c r="F27" t="n">
-        <v>31.5259052367879</v>
+        <v>101988.286173924</v>
       </c>
       <c r="G27" t="n">
-        <v>42.3529078094978</v>
+        <v>134438.946863554</v>
       </c>
       <c r="H27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B28" t="n">
-        <v>1.31151225140582</v>
+        <v>0.8500022449065</v>
       </c>
       <c r="C28" t="n">
-        <v>6.93892473125611</v>
+        <v>0.853354669095716</v>
       </c>
       <c r="D28" t="n">
-        <v>11.4223175159882</v>
+        <v>0.900009615633225</v>
       </c>
       <c r="E28" t="n">
-        <v>11.4301138793729</v>
+        <v>0.900028816412669</v>
       </c>
       <c r="F28" t="n">
-        <v>15.8700177786242</v>
+        <v>0.946639078844455</v>
       </c>
       <c r="G28" t="n">
-        <v>21.093050933684</v>
+        <v>0.949999343883246</v>
       </c>
       <c r="H28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B29" t="n">
-        <v>0.849106505337097</v>
+        <v>-318.655374180954</v>
       </c>
       <c r="C29" t="n">
-        <v>9.74302035463168</v>
+        <v>6.57270762438826</v>
       </c>
       <c r="D29" t="n">
-        <v>16.0454896030748</v>
+        <v>12.3475238737238</v>
       </c>
       <c r="E29" t="n">
-        <v>16.0475730000347</v>
+        <v>11.7293373736918</v>
       </c>
       <c r="F29" t="n">
-        <v>22.3000591341678</v>
+        <v>21.7787148473944</v>
       </c>
       <c r="G29" t="n">
-        <v>31.466853048242</v>
+        <v>98.2231377396377</v>
       </c>
       <c r="H29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B30" t="n">
-        <v>0.00707543902837554</v>
+        <v>0.0123912599147962</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0224787327061867</v>
+        <v>0.0188249897333742</v>
       </c>
       <c r="D30" t="n">
-        <v>0.040456910565085</v>
+        <v>0.0328407066411762</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0385845833526863</v>
+        <v>0.0310485529882564</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0695820549394202</v>
+        <v>0.0570769177690416</v>
       </c>
       <c r="G30" t="n">
-        <v>0.509508910007306</v>
+        <v>6.92089023218788</v>
       </c>
       <c r="H30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B31" t="n">
-        <v>7160.34658065747</v>
+        <v>16366.6622391979</v>
       </c>
       <c r="C31" t="n">
-        <v>40976.1115702411</v>
+        <v>27307.7683558608</v>
       </c>
       <c r="D31" t="n">
-        <v>69792.8388893472</v>
+        <v>45048.6253765035</v>
       </c>
       <c r="E31" t="n">
-        <v>69081.2913253985</v>
+        <v>43871.4800927683</v>
       </c>
       <c r="F31" t="n">
-        <v>102597.104389054</v>
+        <v>69067.4372256124</v>
       </c>
       <c r="G31" t="n">
-        <v>143795.177681561</v>
+        <v>102213.692282466</v>
       </c>
       <c r="H31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B32" t="n">
-        <v>0.574510276000798</v>
+        <v>0.850000723684207</v>
       </c>
       <c r="C32" t="n">
-        <v>0.702226154935601</v>
+        <v>0.853310875543393</v>
       </c>
       <c r="D32" t="n">
-        <v>0.799860277654019</v>
+        <v>0.899975627549664</v>
       </c>
       <c r="E32" t="n">
-        <v>0.799605536871719</v>
+        <v>0.900043681333773</v>
       </c>
       <c r="F32" t="n">
-        <v>0.898203826338508</v>
+        <v>0.946560657818918</v>
       </c>
       <c r="G32" t="n">
-        <v>1.02849508019061</v>
+        <v>0.949999961559661</v>
       </c>
       <c r="H32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B33" t="n">
-        <v>2.23161681925784</v>
+        <v>2.55236478048162</v>
       </c>
       <c r="C33" t="n">
-        <v>6.86176452734702</v>
+        <v>5.05776257800928</v>
       </c>
       <c r="D33" t="n">
-        <v>13.7304914799433</v>
+        <v>9.75632518922742</v>
       </c>
       <c r="E33" t="n">
-        <v>13.0227114456162</v>
+        <v>9.16352080366833</v>
       </c>
       <c r="F33" t="n">
-        <v>24.7277327357769</v>
+        <v>17.7383030338704</v>
       </c>
       <c r="G33" t="n">
-        <v>149.813488044006</v>
+        <v>1905.76369706639</v>
       </c>
       <c r="H33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B34" t="n">
-        <v>0.00829017232667438</v>
+        <v>0.01492705443877</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0301425058178134</v>
+        <v>0.0219096203164989</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0541886051359689</v>
+        <v>0.0381768602774448</v>
       </c>
       <c r="E34" t="n">
-        <v>0.0516548168910111</v>
+        <v>0.036136846730656</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0930719432319443</v>
+        <v>0.0660928896746325</v>
       </c>
       <c r="G34" t="n">
-        <v>0.319224064382335</v>
+        <v>0.178544238128866</v>
       </c>
       <c r="H34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B35" t="n">
-        <v>7699.3436596298</v>
+        <v>16000.1483673584</v>
       </c>
       <c r="C35" t="n">
-        <v>32597.4671385319</v>
+        <v>21006.6100155806</v>
       </c>
       <c r="D35" t="n">
-        <v>55360.7479722828</v>
+        <v>33578.2578569923</v>
       </c>
       <c r="E35" t="n">
-        <v>54780.0300138709</v>
+        <v>32690.2927165098</v>
       </c>
       <c r="F35" t="n">
-        <v>81431.3911804832</v>
+        <v>51012.3337022561</v>
       </c>
       <c r="G35" t="n">
-        <v>117745.443063045</v>
+        <v>76768.0467392613</v>
       </c>
       <c r="H35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36" t="n">
-        <v>0.583175114991355</v>
+        <v>0.850000324193388</v>
       </c>
       <c r="C36" t="n">
-        <v>0.701966109414241</v>
+        <v>0.853409620819148</v>
       </c>
       <c r="D36" t="n">
-        <v>0.799996933947921</v>
+        <v>0.899882450858845</v>
       </c>
       <c r="E36" t="n">
-        <v>0.799846249623459</v>
+        <v>0.899748743604869</v>
       </c>
       <c r="F36" t="n">
-        <v>0.898366787954287</v>
+        <v>0.946668707599747</v>
       </c>
       <c r="G36" t="n">
-        <v>1.04708117625778</v>
+        <v>0.949999756016768</v>
       </c>
       <c r="H36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B37" t="n">
-        <v>1.37668731111268</v>
+        <v>2.27777105132891</v>
       </c>
       <c r="C37" t="n">
-        <v>6.78935427032539</v>
+        <v>4.06488270314234</v>
       </c>
       <c r="D37" t="n">
-        <v>13.50991545519</v>
+        <v>7.65102944536932</v>
       </c>
       <c r="E37" t="n">
-        <v>12.8062990176047</v>
+        <v>7.20661041412179</v>
       </c>
       <c r="F37" t="n">
-        <v>24.2798613202566</v>
+        <v>13.8086859955315</v>
       </c>
       <c r="G37" t="n">
-        <v>86.1392234659017</v>
+        <v>37.4154069241203</v>
       </c>
       <c r="H37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0151282574836931</v>
+        <v>0.0160793937979448</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0347917964251265</v>
+        <v>0.0246899177320784</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0624170173829962</v>
+        <v>0.042902803282694</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0594807603856498</v>
+        <v>0.0405797690516301</v>
       </c>
       <c r="F38" t="n">
-        <v>0.107073207178449</v>
+        <v>0.0741752321118128</v>
       </c>
       <c r="G38" t="n">
-        <v>0.735976979442612</v>
+        <v>0.676021185735506</v>
       </c>
       <c r="H38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B39" t="n">
-        <v>6229.28155402082</v>
+        <v>14004.2949339101</v>
       </c>
       <c r="C39" t="n">
-        <v>24887.0711596809</v>
+        <v>17885.2557360079</v>
       </c>
       <c r="D39" t="n">
-        <v>42528.7041601821</v>
+        <v>28373.5980168464</v>
       </c>
       <c r="E39" t="n">
-        <v>42094.7980673464</v>
+        <v>27595.8966911044</v>
       </c>
       <c r="F39" t="n">
-        <v>62681.4716069434</v>
+        <v>42891.6498649898</v>
       </c>
       <c r="G39" t="n">
-        <v>91983.4133652837</v>
+        <v>61848.9121080208</v>
       </c>
       <c r="H39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40" t="n">
-        <v>0.574891759796379</v>
+        <v>0.850000336696394</v>
       </c>
       <c r="C40" t="n">
-        <v>0.702357582463931</v>
+        <v>0.853436073179473</v>
       </c>
       <c r="D40" t="n">
-        <v>0.800151604089351</v>
+        <v>0.900123978960959</v>
       </c>
       <c r="E40" t="n">
-        <v>0.800133342270392</v>
+        <v>0.90010386252543</v>
       </c>
       <c r="F40" t="n">
-        <v>0.897982749499301</v>
+        <v>0.946595108631882</v>
       </c>
       <c r="G40" t="n">
-        <v>1.03005226929108</v>
+        <v>0.949999641929753</v>
       </c>
       <c r="H40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B41" t="n">
-        <v>1.76143373664655</v>
+        <v>2.15641660266297</v>
       </c>
       <c r="C41" t="n">
-        <v>5.48918252158474</v>
+        <v>3.67379397486544</v>
       </c>
       <c r="D41" t="n">
-        <v>10.927726213134</v>
+        <v>6.8877782785652</v>
       </c>
       <c r="E41" t="n">
-        <v>10.3603685736135</v>
+        <v>6.48645374532313</v>
       </c>
       <c r="F41" t="n">
-        <v>19.6238370784973</v>
+        <v>12.3681944338767</v>
       </c>
       <c r="G41" t="n">
-        <v>106.80274146955</v>
+        <v>145.240748983819</v>
       </c>
       <c r="H41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B42" t="n">
-        <v>0.01157743322771</v>
+        <v>-18886.2783115775</v>
       </c>
       <c r="C42" t="n">
-        <v>0.037959308403849</v>
+        <v>370.448509751035</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0684774522082184</v>
+        <v>833.131385183069</v>
       </c>
       <c r="E42" t="n">
-        <v>0.0651622221427841</v>
+        <v>781.764986646168</v>
       </c>
       <c r="F42" t="n">
-        <v>0.117926887623231</v>
+        <v>1600.73210941449</v>
       </c>
       <c r="G42" t="n">
-        <v>9.73698093999048</v>
+        <v>7242.42424724246</v>
       </c>
       <c r="H42" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B43" t="n">
-        <v>5170.41581172019</v>
+        <v>10.2157638170893</v>
       </c>
       <c r="C43" t="n">
-        <v>22831.3241983622</v>
+        <v>95.6727250920814</v>
       </c>
       <c r="D43" t="n">
-        <v>38992.0910790503</v>
+        <v>221.013315383567</v>
       </c>
       <c r="E43" t="n">
-        <v>38620.9051247172</v>
+        <v>204.852909054966</v>
       </c>
       <c r="F43" t="n">
-        <v>57485.0988856455</v>
+        <v>435.443946120915</v>
       </c>
       <c r="G43" t="n">
-        <v>82490.4225985259</v>
+        <v>50704.8994705482</v>
       </c>
       <c r="H43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" t="n">
-        <v>0.591130042648208</v>
+        <v>13.69874795304</v>
       </c>
       <c r="C44" t="n">
-        <v>0.702254363031818</v>
+        <v>38.4207491689144</v>
       </c>
       <c r="D44" t="n">
-        <v>0.799990172781505</v>
+        <v>87.3510238445955</v>
       </c>
       <c r="E44" t="n">
-        <v>0.800048263270451</v>
+        <v>81.3021764637183</v>
       </c>
       <c r="F44" t="n">
-        <v>0.897761865792078</v>
+        <v>170.608054950649</v>
       </c>
       <c r="G44" t="n">
-        <v>1.01656915029827</v>
+        <v>461.356599637686</v>
       </c>
       <c r="H44" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45">
@@ -1567,22 +1564,22 @@
         <v>12</v>
       </c>
       <c r="B45" t="n">
-        <v>1.30551197494169</v>
+        <v>8.70443032084218</v>
       </c>
       <c r="C45" t="n">
-        <v>5.37640879190902</v>
+        <v>49.1438230765531</v>
       </c>
       <c r="D45" t="n">
-        <v>10.6945735101986</v>
+        <v>110.554179072069</v>
       </c>
       <c r="E45" t="n">
-        <v>10.1235320709573</v>
+        <v>102.8993513315</v>
       </c>
       <c r="F45" t="n">
-        <v>19.1417553395268</v>
+        <v>215.629359624807</v>
       </c>
       <c r="G45" t="n">
-        <v>1801.7786001562</v>
+        <v>2919.00789359448</v>
       </c>
       <c r="H45" t="s">
         <v>22</v>
@@ -1593,22 +1590,22 @@
         <v>8</v>
       </c>
       <c r="B46" t="n">
-        <v>98.5838985464683</v>
+        <v>-14513.87240147</v>
       </c>
       <c r="C46" t="n">
-        <v>393.807083592686</v>
+        <v>292.403872128758</v>
       </c>
       <c r="D46" t="n">
-        <v>926.971759008565</v>
+        <v>666.563524648189</v>
       </c>
       <c r="E46" t="n">
-        <v>867.192059905529</v>
+        <v>623.827467399707</v>
       </c>
       <c r="F46" t="n">
-        <v>1815.15014956513</v>
+        <v>1292.87133657941</v>
       </c>
       <c r="G46" t="n">
-        <v>14784.6077020417</v>
+        <v>5605.54639654149</v>
       </c>
       <c r="H46" t="s">
         <v>23</v>
@@ -1619,22 +1616,22 @@
         <v>10</v>
       </c>
       <c r="B47" t="n">
-        <v>29.6253032698613</v>
+        <v>7.87831812123685</v>
       </c>
       <c r="C47" t="n">
-        <v>129.745076297747</v>
+        <v>75.4822667448007</v>
       </c>
       <c r="D47" t="n">
-        <v>305.767523041469</v>
+        <v>176.722270374039</v>
       </c>
       <c r="E47" t="n">
-        <v>286.043969392322</v>
+        <v>163.50636083723</v>
       </c>
       <c r="F47" t="n">
-        <v>594.675633507276</v>
+        <v>351.49741924074</v>
       </c>
       <c r="G47" t="n">
-        <v>2360.78894886615</v>
+        <v>39287.7269496013</v>
       </c>
       <c r="H47" t="s">
         <v>23</v>
@@ -1645,22 +1642,22 @@
         <v>11</v>
       </c>
       <c r="B48" t="n">
-        <v>12.4673230049814</v>
+        <v>10.343039426137</v>
       </c>
       <c r="C48" t="n">
-        <v>52.9402006529695</v>
+        <v>30.2866009660142</v>
       </c>
       <c r="D48" t="n">
-        <v>124.85412113909</v>
+        <v>69.8804847224142</v>
       </c>
       <c r="E48" t="n">
-        <v>116.791477748783</v>
+        <v>64.8917817516548</v>
       </c>
       <c r="F48" t="n">
-        <v>243.358909267063</v>
+        <v>138.021307978172</v>
       </c>
       <c r="G48" t="n">
-        <v>1526.76990171578</v>
+        <v>408.334333004727</v>
       </c>
       <c r="H48" t="s">
         <v>23</v>
@@ -1671,129 +1668,25 @@
         <v>12</v>
       </c>
       <c r="B49" t="n">
-        <v>6.63252369385525</v>
+        <v>6.74558957517604</v>
       </c>
       <c r="C49" t="n">
-        <v>73.2061744487878</v>
+        <v>38.6258993110005</v>
       </c>
       <c r="D49" t="n">
-        <v>171.643481706038</v>
+        <v>88.4903290208524</v>
       </c>
       <c r="E49" t="n">
-        <v>160.071361371485</v>
+        <v>82.1081349367199</v>
       </c>
       <c r="F49" t="n">
-        <v>334.156612167944</v>
+        <v>174.573432947894</v>
       </c>
       <c r="G49" t="n">
-        <v>33985.6263055642</v>
+        <v>2243.40775350366</v>
       </c>
       <c r="H49" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" t="n">
-        <v>82.3184570004929</v>
-      </c>
-      <c r="C50" t="n">
-        <v>310.213892792949</v>
-      </c>
-      <c r="D50" t="n">
-        <v>741.725961210241</v>
-      </c>
-      <c r="E50" t="n">
-        <v>691.592158829535</v>
-      </c>
-      <c r="F50" t="n">
-        <v>1469.25586632349</v>
-      </c>
-      <c r="G50" t="n">
-        <v>11150.7587000077</v>
-      </c>
-      <c r="H50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
-        <v>10</v>
-      </c>
-      <c r="B51" t="n">
-        <v>21.8091567045101</v>
-      </c>
-      <c r="C51" t="n">
-        <v>102.440115523671</v>
-      </c>
-      <c r="D51" t="n">
-        <v>244.603301497844</v>
-      </c>
-      <c r="E51" t="n">
-        <v>228.248898975518</v>
-      </c>
-      <c r="F51" t="n">
-        <v>482.053571236481</v>
-      </c>
-      <c r="G51" t="n">
-        <v>1998.04245514958</v>
-      </c>
-      <c r="H51" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" t="n">
-        <v>9.11113064509024</v>
-      </c>
-      <c r="C52" t="n">
-        <v>41.7884204690033</v>
-      </c>
-      <c r="D52" t="n">
-        <v>99.9001023265774</v>
-      </c>
-      <c r="E52" t="n">
-        <v>93.158248596458</v>
-      </c>
-      <c r="F52" t="n">
-        <v>197.044048607133</v>
-      </c>
-      <c r="G52" t="n">
-        <v>1294.09084776918</v>
-      </c>
-      <c r="H52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B53" t="n">
-        <v>5.48143244825728</v>
-      </c>
-      <c r="C53" t="n">
-        <v>57.6567174310718</v>
-      </c>
-      <c r="D53" t="n">
-        <v>137.321125592634</v>
-      </c>
-      <c r="E53" t="n">
-        <v>127.802295865969</v>
-      </c>
-      <c r="F53" t="n">
-        <v>269.431470265602</v>
-      </c>
-      <c r="G53" t="n">
-        <v>26597.5260846402</v>
-      </c>
-      <c r="H53" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A few figures settings
</commit_message>
<xml_diff>
--- a/output/supp_mat1.xlsx
+++ b/output/supp_mat1.xlsx
@@ -404,22 +404,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>0.582312245481221</v>
+        <v>0.586529631431128</v>
       </c>
       <c r="C2" t="n">
-        <v>2.31174574942257</v>
+        <v>2.34673203624268</v>
       </c>
       <c r="D2" t="n">
-        <v>9.71846063957016</v>
+        <v>9.85205052555044</v>
       </c>
       <c r="E2" t="n">
-        <v>8.44423096866041</v>
+        <v>8.56199199560445</v>
       </c>
       <c r="F2" t="n">
-        <v>24.427811206171</v>
+        <v>24.8357787251713</v>
       </c>
       <c r="G2" t="n">
-        <v>100.312929246159</v>
+        <v>112.655079032719</v>
       </c>
     </row>
     <row r="3">
@@ -427,22 +427,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>3.75402348695717</v>
+        <v>3.97357582083055</v>
       </c>
       <c r="C3" t="n">
-        <v>12.3523395214045</v>
+        <v>12.4981671203927</v>
       </c>
       <c r="D3" t="n">
-        <v>43.5372812714913</v>
+        <v>44.1331234693127</v>
       </c>
       <c r="E3" t="n">
-        <v>38.4957567164209</v>
+        <v>39.0376136440094</v>
       </c>
       <c r="F3" t="n">
-        <v>103.408058751747</v>
+        <v>105.158312520551</v>
       </c>
       <c r="G3" t="n">
-        <v>392.685850239176</v>
+        <v>420.176226541882</v>
       </c>
     </row>
     <row r="4">
@@ -450,22 +450,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>17.0056341062422</v>
+        <v>15.9268883994592</v>
       </c>
       <c r="C4" t="n">
-        <v>59.1151022823119</v>
+        <v>59.7519840083259</v>
       </c>
       <c r="D4" t="n">
-        <v>149.464993029533</v>
+        <v>151.526108843887</v>
       </c>
       <c r="E4" t="n">
-        <v>137.096776986925</v>
+        <v>138.760678899159</v>
       </c>
       <c r="F4" t="n">
-        <v>311.316952676775</v>
+        <v>316.049699767064</v>
       </c>
       <c r="G4" t="n">
-        <v>850.990988524279</v>
+        <v>873.360947442294</v>
       </c>
     </row>
     <row r="5">
@@ -473,22 +473,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>0.255033144765084</v>
+        <v>0.25763596286562</v>
       </c>
       <c r="C5" t="n">
-        <v>0.932014984439093</v>
+        <v>0.940934258559688</v>
       </c>
       <c r="D5" t="n">
-        <v>3.08947832460019</v>
+        <v>3.13211817419696</v>
       </c>
       <c r="E5" t="n">
-        <v>2.69396590295945</v>
+        <v>2.73058854604128</v>
       </c>
       <c r="F5" t="n">
-        <v>7.51138324483634</v>
+        <v>7.63142934780946</v>
       </c>
       <c r="G5" t="n">
-        <v>25.0156050214649</v>
+        <v>25.7236493510681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>